<commit_message>
Updated Sprint Backlog from sprint 4 Updated Scrum Board and Work Breakdown Structure from the Project
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint 4/Sprint Backlog.xlsx
+++ b/Project/Phase 2/Sprint 4/Sprint Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\Documents\GanttProject\Project\Phase 2\Sprint 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4750289-ED03-444C-B3FE-C68C2E81B1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE53FD1F-3E76-4DB7-887D-3BC61CAC1DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8105ECB6-96AF-4B3F-9441-D4A4BE61F8E3}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,10 +535,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2"/>
       <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
@@ -547,11 +547,11 @@
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="2"/>
       <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
@@ -560,11 +560,11 @@
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
       <c r="E6" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>